<commit_message>
Updated powerpoint statistics for Doubles 2023
</commit_message>
<xml_diff>
--- a/exports/matches_table.xlsx
+++ b/exports/matches_table.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V98"/>
+  <dimension ref="A1:V112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3086,7 +3086,7 @@
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Sam Carswell-Tellis</t>
+          <t>Sam Tellis</t>
         </is>
       </c>
       <c r="I38" t="inlineStr"/>
@@ -3290,7 +3290,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Levin Lee</t>
+          <t>Kevin Lee</t>
         </is>
       </c>
       <c r="G41" t="inlineStr"/>
@@ -3500,7 +3500,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Sam Carswell-Tellis</t>
+          <t>Sam Tellis</t>
         </is>
       </c>
       <c r="G44" t="inlineStr"/>
@@ -4060,7 +4060,7 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Levin Lee</t>
+          <t>Kevin Lee</t>
         </is>
       </c>
       <c r="G52" t="inlineStr"/>
@@ -4626,7 +4626,7 @@
       <c r="G60" t="inlineStr"/>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Levin Lee</t>
+          <t>Kevin Lee</t>
         </is>
       </c>
       <c r="I60" t="inlineStr"/>
@@ -4906,7 +4906,7 @@
       <c r="G64" t="inlineStr"/>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Levin Lee</t>
+          <t>Kevin Lee</t>
         </is>
       </c>
       <c r="I64" t="inlineStr"/>
@@ -5040,7 +5040,7 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Levin Lee</t>
+          <t>Kevin Lee</t>
         </is>
       </c>
       <c r="G66" t="inlineStr"/>
@@ -5116,7 +5116,7 @@
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Levin Lee</t>
+          <t>Kevin Lee</t>
         </is>
       </c>
       <c r="I67" t="inlineStr"/>
@@ -5419,7 +5419,7 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>Levin Lee</t>
+          <t>Kevin Lee</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
@@ -5741,7 +5741,7 @@
       </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t>Levin Lee</t>
+          <t>Kevin Lee</t>
         </is>
       </c>
       <c r="J75" t="n">
@@ -6053,7 +6053,7 @@
       </c>
       <c r="I79" t="inlineStr">
         <is>
-          <t>Levin Lee</t>
+          <t>Kevin Lee</t>
         </is>
       </c>
       <c r="J79" t="n">
@@ -6121,7 +6121,7 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>Levin Lee</t>
+          <t>Kevin Lee</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
@@ -6209,7 +6209,7 @@
       </c>
       <c r="I81" t="inlineStr">
         <is>
-          <t>Levin Lee</t>
+          <t>Kevin Lee</t>
         </is>
       </c>
       <c r="J81" t="n">
@@ -6589,7 +6589,7 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>Levin Lee</t>
+          <t>Kevin Lee</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
@@ -6979,7 +6979,7 @@
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>Levin Lee</t>
+          <t>Kevin Lee</t>
         </is>
       </c>
       <c r="H91" t="inlineStr">
@@ -7291,7 +7291,7 @@
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>Levin Lee</t>
+          <t>Kevin Lee</t>
         </is>
       </c>
       <c r="H95" t="inlineStr">
@@ -7369,7 +7369,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>Levin Lee</t>
+          <t>Kevin Lee</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
@@ -7457,7 +7457,7 @@
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>Levin Lee</t>
+          <t>Kevin Lee</t>
         </is>
       </c>
       <c r="J97" t="n">
@@ -7535,7 +7535,7 @@
       </c>
       <c r="I98" t="inlineStr">
         <is>
-          <t>Levin Lee</t>
+          <t>Kevin Lee</t>
         </is>
       </c>
       <c r="J98" t="n">
@@ -7576,6 +7576,1098 @@
       </c>
       <c r="V98" t="n">
         <v>0.2936507936507936</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>2023_2s</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>1</v>
+      </c>
+      <c r="D99" t="b">
+        <v>0</v>
+      </c>
+      <c r="E99" t="b">
+        <v>0</v>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>Rohan Chowla</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>Kevin Lee</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>Noah Dale</t>
+        </is>
+      </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>Yafu LastName</t>
+        </is>
+      </c>
+      <c r="J99" t="n">
+        <v>6</v>
+      </c>
+      <c r="K99" t="n">
+        <v>5</v>
+      </c>
+      <c r="L99" t="n">
+        <v>1</v>
+      </c>
+      <c r="M99" t="n">
+        <v>8</v>
+      </c>
+      <c r="N99" t="n">
+        <v>6</v>
+      </c>
+      <c r="O99" t="n">
+        <v>-7</v>
+      </c>
+      <c r="P99" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q99" t="n">
+        <v>50</v>
+      </c>
+      <c r="R99" t="n">
+        <v>50</v>
+      </c>
+      <c r="S99" t="n">
+        <v>-1</v>
+      </c>
+      <c r="T99" t="n">
+        <v>-0.1666666666666667</v>
+      </c>
+      <c r="U99" t="n">
+        <v>-0.1666666666666667</v>
+      </c>
+      <c r="V99" t="n">
+        <v>0.1666666666666667</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>2023_2s</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>2</v>
+      </c>
+      <c r="D100" t="b">
+        <v>0</v>
+      </c>
+      <c r="E100" t="b">
+        <v>0</v>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>Gabe Silverstein</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>Alex LastName</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>Luci Nguyen</t>
+        </is>
+      </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>Matthew Rusten</t>
+        </is>
+      </c>
+      <c r="J100" t="n">
+        <v>3</v>
+      </c>
+      <c r="K100" t="n">
+        <v>6</v>
+      </c>
+      <c r="L100" t="n">
+        <v>4</v>
+      </c>
+      <c r="M100" t="n">
+        <v>5</v>
+      </c>
+      <c r="N100" t="n">
+        <v>6</v>
+      </c>
+      <c r="O100" t="n">
+        <v>-1</v>
+      </c>
+      <c r="P100" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q100" t="n">
+        <v>50</v>
+      </c>
+      <c r="R100" t="n">
+        <v>50</v>
+      </c>
+      <c r="S100" t="n">
+        <v>3</v>
+      </c>
+      <c r="T100" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="U100" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="V100" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>2023_2s</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>3</v>
+      </c>
+      <c r="D101" t="b">
+        <v>0</v>
+      </c>
+      <c r="E101" t="b">
+        <v>0</v>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>Cason Duszak</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>Eric LastName</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>Piper Parker</t>
+        </is>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>Kim LastName</t>
+        </is>
+      </c>
+      <c r="J101" t="n">
+        <v>6</v>
+      </c>
+      <c r="K101" t="n">
+        <v>3</v>
+      </c>
+      <c r="L101" t="n">
+        <v>2</v>
+      </c>
+      <c r="M101" t="n">
+        <v>7</v>
+      </c>
+      <c r="N101" t="n">
+        <v>6</v>
+      </c>
+      <c r="O101" t="n">
+        <v>-5</v>
+      </c>
+      <c r="P101" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q101" t="n">
+        <v>50</v>
+      </c>
+      <c r="R101" t="n">
+        <v>50</v>
+      </c>
+      <c r="S101" t="n">
+        <v>-3</v>
+      </c>
+      <c r="T101" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="U101" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="V101" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>2023_2s</t>
+        </is>
+      </c>
+      <c r="C102" t="n">
+        <v>4</v>
+      </c>
+      <c r="D102" t="b">
+        <v>0</v>
+      </c>
+      <c r="E102" t="b">
+        <v>0</v>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>Nathan Snow</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>Jason Jackson</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>Julie Jackson</t>
+        </is>
+      </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>Carolyn LastName</t>
+        </is>
+      </c>
+      <c r="J102" t="n">
+        <v>6</v>
+      </c>
+      <c r="K102" t="n">
+        <v>4</v>
+      </c>
+      <c r="L102" t="n">
+        <v>3</v>
+      </c>
+      <c r="M102" t="n">
+        <v>6</v>
+      </c>
+      <c r="N102" t="n">
+        <v>6</v>
+      </c>
+      <c r="O102" t="n">
+        <v>-3</v>
+      </c>
+      <c r="P102" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q102" t="n">
+        <v>50</v>
+      </c>
+      <c r="R102" t="n">
+        <v>50</v>
+      </c>
+      <c r="S102" t="n">
+        <v>-2</v>
+      </c>
+      <c r="T102" t="n">
+        <v>-0.3333333333333333</v>
+      </c>
+      <c r="U102" t="n">
+        <v>-0.3333333333333333</v>
+      </c>
+      <c r="V102" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>2023_2s</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>5</v>
+      </c>
+      <c r="D103" t="b">
+        <v>1</v>
+      </c>
+      <c r="E103" t="b">
+        <v>1</v>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>Noah Dale</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>Yafu LastName</t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>Gabe Silverstein</t>
+        </is>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>Alex LastName</t>
+        </is>
+      </c>
+      <c r="J103" t="n">
+        <v>5</v>
+      </c>
+      <c r="K103" t="n">
+        <v>6</v>
+      </c>
+      <c r="L103" t="n">
+        <v>8</v>
+      </c>
+      <c r="M103" t="n">
+        <v>4</v>
+      </c>
+      <c r="N103" t="n">
+        <v>6</v>
+      </c>
+      <c r="O103" t="n">
+        <v>4</v>
+      </c>
+      <c r="P103" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q103" t="n">
+        <v>50</v>
+      </c>
+      <c r="R103" t="n">
+        <v>50</v>
+      </c>
+      <c r="S103" t="n">
+        <v>1</v>
+      </c>
+      <c r="T103" t="n">
+        <v>0.1666666666666667</v>
+      </c>
+      <c r="U103" t="n">
+        <v>0.1666666666666667</v>
+      </c>
+      <c r="V103" t="n">
+        <v>0.1666666666666667</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>2023_2s</t>
+        </is>
+      </c>
+      <c r="C104" t="n">
+        <v>6</v>
+      </c>
+      <c r="D104" t="b">
+        <v>1</v>
+      </c>
+      <c r="E104" t="b">
+        <v>1</v>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>Piper Parker</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>Kim LastName</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>Julie Jackson</t>
+        </is>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>Carolyn LastName</t>
+        </is>
+      </c>
+      <c r="J104" t="n">
+        <v>2</v>
+      </c>
+      <c r="K104" t="n">
+        <v>6</v>
+      </c>
+      <c r="L104" t="n">
+        <v>7</v>
+      </c>
+      <c r="M104" t="n">
+        <v>6</v>
+      </c>
+      <c r="N104" t="n">
+        <v>6</v>
+      </c>
+      <c r="O104" t="n">
+        <v>1</v>
+      </c>
+      <c r="P104" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q104" t="n">
+        <v>50</v>
+      </c>
+      <c r="R104" t="n">
+        <v>50</v>
+      </c>
+      <c r="S104" t="n">
+        <v>4</v>
+      </c>
+      <c r="T104" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="U104" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="V104" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>103</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>2023_2s</t>
+        </is>
+      </c>
+      <c r="C105" t="n">
+        <v>7</v>
+      </c>
+      <c r="D105" t="b">
+        <v>0</v>
+      </c>
+      <c r="E105" t="b">
+        <v>0</v>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>Rohan Chowla</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>Kevin Lee</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>Luci Nguyen</t>
+        </is>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>Matthew Rusten</t>
+        </is>
+      </c>
+      <c r="J105" t="n">
+        <v>6</v>
+      </c>
+      <c r="K105" t="n">
+        <v>2</v>
+      </c>
+      <c r="L105" t="n">
+        <v>1</v>
+      </c>
+      <c r="M105" t="n">
+        <v>5</v>
+      </c>
+      <c r="N105" t="n">
+        <v>6</v>
+      </c>
+      <c r="O105" t="n">
+        <v>-4</v>
+      </c>
+      <c r="P105" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q105" t="n">
+        <v>50</v>
+      </c>
+      <c r="R105" t="n">
+        <v>50</v>
+      </c>
+      <c r="S105" t="n">
+        <v>-4</v>
+      </c>
+      <c r="T105" t="n">
+        <v>-0.6666666666666666</v>
+      </c>
+      <c r="U105" t="n">
+        <v>-0.6666666666666666</v>
+      </c>
+      <c r="V105" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>2023_2s</t>
+        </is>
+      </c>
+      <c r="C106" t="n">
+        <v>8</v>
+      </c>
+      <c r="D106" t="b">
+        <v>0</v>
+      </c>
+      <c r="E106" t="b">
+        <v>0</v>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>Cason Duszak</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>Eric LastName</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>Nathan Snow</t>
+        </is>
+      </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>Jason Jackson</t>
+        </is>
+      </c>
+      <c r="J106" t="n">
+        <v>6</v>
+      </c>
+      <c r="K106" t="n">
+        <v>5</v>
+      </c>
+      <c r="L106" t="n">
+        <v>2</v>
+      </c>
+      <c r="M106" t="n">
+        <v>3</v>
+      </c>
+      <c r="N106" t="n">
+        <v>6</v>
+      </c>
+      <c r="O106" t="n">
+        <v>-1</v>
+      </c>
+      <c r="P106" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q106" t="n">
+        <v>50</v>
+      </c>
+      <c r="R106" t="n">
+        <v>50</v>
+      </c>
+      <c r="S106" t="n">
+        <v>-1</v>
+      </c>
+      <c r="T106" t="n">
+        <v>-0.1666666666666667</v>
+      </c>
+      <c r="U106" t="n">
+        <v>-0.1666666666666667</v>
+      </c>
+      <c r="V106" t="n">
+        <v>0.1666666666666667</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>2023_2s</t>
+        </is>
+      </c>
+      <c r="C107" t="n">
+        <v>9</v>
+      </c>
+      <c r="D107" t="b">
+        <v>1</v>
+      </c>
+      <c r="E107" t="b">
+        <v>1</v>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>Luci Nguyen</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>Matthew Rusten</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>Julie Jackson</t>
+        </is>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>Carolyn LastName</t>
+        </is>
+      </c>
+      <c r="J107" t="n">
+        <v>6</v>
+      </c>
+      <c r="K107" t="n">
+        <v>5</v>
+      </c>
+      <c r="L107" t="n">
+        <v>5</v>
+      </c>
+      <c r="M107" t="n">
+        <v>6</v>
+      </c>
+      <c r="N107" t="n">
+        <v>6</v>
+      </c>
+      <c r="O107" t="n">
+        <v>-1</v>
+      </c>
+      <c r="P107" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q107" t="n">
+        <v>50</v>
+      </c>
+      <c r="R107" t="n">
+        <v>50</v>
+      </c>
+      <c r="S107" t="n">
+        <v>-1</v>
+      </c>
+      <c r="T107" t="n">
+        <v>-0.1666666666666667</v>
+      </c>
+      <c r="U107" t="n">
+        <v>-0.1666666666666667</v>
+      </c>
+      <c r="V107" t="n">
+        <v>0.1666666666666667</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>2023_2s</t>
+        </is>
+      </c>
+      <c r="C108" t="n">
+        <v>10</v>
+      </c>
+      <c r="D108" t="b">
+        <v>1</v>
+      </c>
+      <c r="E108" t="b">
+        <v>1</v>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>Nathan Snow</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>Jason Jackson</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>Gabe Silverstein</t>
+        </is>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>Alex LastName</t>
+        </is>
+      </c>
+      <c r="J108" t="n">
+        <v>6</v>
+      </c>
+      <c r="K108" t="n">
+        <v>5</v>
+      </c>
+      <c r="L108" t="n">
+        <v>3</v>
+      </c>
+      <c r="M108" t="n">
+        <v>4</v>
+      </c>
+      <c r="N108" t="n">
+        <v>6</v>
+      </c>
+      <c r="O108" t="n">
+        <v>-1</v>
+      </c>
+      <c r="P108" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q108" t="n">
+        <v>50</v>
+      </c>
+      <c r="R108" t="n">
+        <v>50</v>
+      </c>
+      <c r="S108" t="n">
+        <v>-1</v>
+      </c>
+      <c r="T108" t="n">
+        <v>-0.1666666666666667</v>
+      </c>
+      <c r="U108" t="n">
+        <v>-0.1666666666666667</v>
+      </c>
+      <c r="V108" t="n">
+        <v>0.1666666666666667</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>2023_2s</t>
+        </is>
+      </c>
+      <c r="C109" t="n">
+        <v>11</v>
+      </c>
+      <c r="D109" t="b">
+        <v>1</v>
+      </c>
+      <c r="E109" t="b">
+        <v>1</v>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>Nathan Snow</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>Jason Jackson</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>Luci Nguyen</t>
+        </is>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>Matthew Rusten</t>
+        </is>
+      </c>
+      <c r="J109" t="n">
+        <v>9</v>
+      </c>
+      <c r="K109" t="n">
+        <v>7</v>
+      </c>
+      <c r="L109" t="n">
+        <v>3</v>
+      </c>
+      <c r="M109" t="n">
+        <v>5</v>
+      </c>
+      <c r="N109" t="n">
+        <v>9</v>
+      </c>
+      <c r="O109" t="n">
+        <v>-2</v>
+      </c>
+      <c r="P109" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q109" t="n">
+        <v>50</v>
+      </c>
+      <c r="R109" t="n">
+        <v>50</v>
+      </c>
+      <c r="S109" t="n">
+        <v>-2</v>
+      </c>
+      <c r="T109" t="n">
+        <v>-0.3333333333333333</v>
+      </c>
+      <c r="U109" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="V109" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>2023_2s</t>
+        </is>
+      </c>
+      <c r="C110" t="n">
+        <v>12</v>
+      </c>
+      <c r="D110" t="b">
+        <v>0</v>
+      </c>
+      <c r="E110" t="b">
+        <v>0</v>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>Rohan Chowla</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>Kevin Lee</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>Cason Duszak</t>
+        </is>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>Eric LastName</t>
+        </is>
+      </c>
+      <c r="J110" t="n">
+        <v>6</v>
+      </c>
+      <c r="K110" t="n">
+        <v>5</v>
+      </c>
+      <c r="L110" t="n">
+        <v>1</v>
+      </c>
+      <c r="M110" t="n">
+        <v>2</v>
+      </c>
+      <c r="N110" t="n">
+        <v>6</v>
+      </c>
+      <c r="O110" t="n">
+        <v>-1</v>
+      </c>
+      <c r="P110" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q110" t="n">
+        <v>50</v>
+      </c>
+      <c r="R110" t="n">
+        <v>50</v>
+      </c>
+      <c r="S110" t="n">
+        <v>-1</v>
+      </c>
+      <c r="T110" t="n">
+        <v>-0.1666666666666667</v>
+      </c>
+      <c r="U110" t="n">
+        <v>-0.1666666666666667</v>
+      </c>
+      <c r="V110" t="n">
+        <v>0.1666666666666667</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>109</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>2023_2s</t>
+        </is>
+      </c>
+      <c r="C111" t="n">
+        <v>13</v>
+      </c>
+      <c r="D111" t="b">
+        <v>1</v>
+      </c>
+      <c r="E111" t="b">
+        <v>1</v>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>Cason Duszak</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>Eric LastName</t>
+        </is>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>Nathan Snow</t>
+        </is>
+      </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>Jason Jackson</t>
+        </is>
+      </c>
+      <c r="J111" t="n">
+        <v>6</v>
+      </c>
+      <c r="K111" t="n">
+        <v>5</v>
+      </c>
+      <c r="L111" t="n">
+        <v>2</v>
+      </c>
+      <c r="M111" t="n">
+        <v>3</v>
+      </c>
+      <c r="N111" t="n">
+        <v>6</v>
+      </c>
+      <c r="O111" t="n">
+        <v>-1</v>
+      </c>
+      <c r="P111" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q111" t="n">
+        <v>50</v>
+      </c>
+      <c r="R111" t="n">
+        <v>50</v>
+      </c>
+      <c r="S111" t="n">
+        <v>-1</v>
+      </c>
+      <c r="T111" t="n">
+        <v>-0.1666666666666667</v>
+      </c>
+      <c r="U111" t="n">
+        <v>-0.1666666666666667</v>
+      </c>
+      <c r="V111" t="n">
+        <v>0.1666666666666667</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>2023_2s</t>
+        </is>
+      </c>
+      <c r="C112" t="n">
+        <v>14</v>
+      </c>
+      <c r="D112" t="b">
+        <v>0</v>
+      </c>
+      <c r="E112" t="b">
+        <v>1</v>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>Rohan Chowla</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>Kevin Lee</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>Cason Duszak</t>
+        </is>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>Eric LastName</t>
+        </is>
+      </c>
+      <c r="J112" t="n">
+        <v>9</v>
+      </c>
+      <c r="K112" t="n">
+        <v>8</v>
+      </c>
+      <c r="L112" t="n">
+        <v>1</v>
+      </c>
+      <c r="M112" t="n">
+        <v>2</v>
+      </c>
+      <c r="N112" t="n">
+        <v>9</v>
+      </c>
+      <c r="O112" t="n">
+        <v>-1</v>
+      </c>
+      <c r="P112" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q112" t="n">
+        <v>50</v>
+      </c>
+      <c r="R112" t="n">
+        <v>50</v>
+      </c>
+      <c r="S112" t="n">
+        <v>-1</v>
+      </c>
+      <c r="T112" t="n">
+        <v>-0.1666666666666667</v>
+      </c>
+      <c r="U112" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="V112" t="n">
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>